<commit_message>
Added Skili jar file and used jxl for excel
</commit_message>
<xml_diff>
--- a/src/main/java/MavenSam/Mavensample/Datatest.xlsx
+++ b/src/main/java/MavenSam/Mavensample/Datatest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -54,10 +54,34 @@
     <t>Taxi</t>
   </si>
   <si>
-    <t>Drivers</t>
-  </si>
-  <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>Doctor appointment</t>
+  </si>
+  <si>
+    <t>Ram10</t>
+  </si>
+  <si>
+    <t>Pawan10</t>
+  </si>
+  <si>
+    <t>Pawan11</t>
+  </si>
+  <si>
+    <t>Ram11</t>
+  </si>
+  <si>
+    <t>Pawan12</t>
+  </si>
+  <si>
+    <t>Ram12</t>
+  </si>
+  <si>
+    <t>Pawan13</t>
+  </si>
+  <si>
+    <t>Ram13</t>
   </si>
   <si>
     <t>Pass</t>
@@ -67,7 +91,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -97,25 +120,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,73 +446,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.400390625" collapsed="false"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2">
+        <v>90256985424</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2">
+        <v>90256985421</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>403373036</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2">
+        <v>90256985418</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3">
-        <v>4025215</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2">
+        <v>90256985415</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="D4" s="1"/>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2">
+        <v>90256985412</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2">
+        <v>90256985409</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2">
+        <v>90256985406</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2">
+        <v>90256985403</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -494,21 +626,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
@@ -516,35 +648,35 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>403373036</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>4025215</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="D4" s="2"/>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>